<commit_message>
Cambio en el libro 01
</commit_message>
<xml_diff>
--- a/lab01/Libro1.xlsx
+++ b/lab01/Libro1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reposInventario2025\lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recuperadoInstructorQuevedo\reposInventario2025\lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAAF38DC-6E7A-48D7-9DD8-ABE7A7A2C7C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F61D9E-66FE-4EE5-9E90-3360E30B8CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4770" yWindow="2445" windowWidth="21600" windowHeight="11295" xr2:uid="{2CBF6FFA-8719-440B-9FC5-C5276456B4AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2CBF6FFA-8719-440B-9FC5-C5276456B4AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -50,13 +50,13 @@
     <t>l001</t>
   </si>
   <si>
-    <t>PC DELL ALL IN ONE CORE I7</t>
-  </si>
-  <si>
     <t>l002</t>
   </si>
   <si>
     <t>l003</t>
+  </si>
+  <si>
+    <t>ola</t>
   </si>
 </sst>
 </file>
@@ -464,29 +464,29 @@
         <v>5445644</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>5885644</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>5445622</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>